<commit_message>
all_args_here small print bug fixed in on.exit()
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE230D52-6B15-4191-9F9E-7FD12BB7ADF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D77BA8-47DF-4292-B42F-053F463B3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -491,7 +491,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -524,6 +524,9 @@
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
.extract_all_fun_names updated with BACKBONE v10.6
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D77BA8-47DF-4292-B42F-053F463B3467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2B2AB8-725D-4A1F-8636-6E935EFCBD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="20330" yWindow="-15150" windowWidth="26740" windowHeight="14930" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Unit tests</t>
+  </si>
+  <si>
+    <t>compare with .colons_check_message</t>
   </si>
 </sst>
 </file>
@@ -491,13 +494,13 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="2"/>
     <col min="5" max="16384" width="11.42578125" style="1"/>
@@ -524,9 +527,6 @@
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -562,12 +562,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -588,6 +588,9 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -643,6 +646,9 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all_args_here BACKBONE v10.7 check TODO
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DE05F2-3875-4189-9861-3A487988E66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AED30E7-16AB-496A-A9E7-B5CC01D41885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20330" yWindow="-15150" windowWidth="26740" windowHeight="14930" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -114,6 +114,47 @@
   </si>
   <si>
     <t>compare with .colons_check_message</t>
+  </si>
+  <si>
+    <t>BACKBONE v10.7</t>
+  </si>
+  <si>
+    <t>71
+error EMPTY</t>
+  </si>
+  <si>
+    <t>76
+error_text = embed</t>
+  </si>
+  <si>
+    <t>59
+error message end by .</t>
+  </si>
+  <si>
+    <t>77
+sub(pattern = "^ERROR IN "</t>
+  </si>
+  <si>
+    <t>78
+internal fun no arg_check -&gt; deal with ""</t>
+  </si>
+  <si>
+    <t>79
+required function fill in internal</t>
+  </si>
+  <si>
+    <t>81
+internal errors number</t>
+  </si>
+  <si>
+    <t>80
+. preceeded by :::</t>
+  </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>check lib_path = lib_path or not</t>
   </si>
 </sst>
 </file>
@@ -491,33 +532,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="14" width="9.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,147 +598,236 @@
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D18" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
.base_op_check BACKBONE v10.7 and check TODO done
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AED30E7-16AB-496A-A9E7-B5CC01D41885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1868EF-A1CE-4A71-8C9D-127C201E5BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -535,7 +535,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -690,10 +690,34 @@
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N9" s="2" t="s">

</xml_diff>

<commit_message>
.pack_and_function_check BACKBONE v10.7 and check TODO done
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1868EF-A1CE-4A71-8C9D-127C201E5BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4017AB1B-80C7-486C-B3C3-6014237D39FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -535,7 +535,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -576,10 +576,10 @@
         <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>36</v>
@@ -619,7 +619,7 @@
       <c r="J2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -720,6 +720,9 @@
       <c r="L9" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="M9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="N9" s="2" t="s">
         <v>23</v>
       </c>
@@ -801,10 +804,37 @@
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N18" s="2" t="s">

</xml_diff>

<commit_message>
.extract_all_fun_names BACKBONE v10.7 and check TODO done
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4017AB1B-80C7-486C-B3C3-6014237D39FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8F0014-08E0-4D1F-8512-5D71A6EE113D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -535,7 +535,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,37 @@
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.noclean_functions BACKBONE v10.7 and check TODO done except all_args_here because bloqued
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8F0014-08E0-4D1F-8512-5D71A6EE113D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4D431-A5FB-4784-AC33-C527C3378824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -147,14 +147,21 @@
 internal errors number</t>
   </si>
   <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>check lib_path = lib_path or not</t>
+  </si>
+  <si>
     <t>80
-. preceeded by :::</t>
-  </si>
-  <si>
-    <t>nc</t>
-  </si>
-  <si>
-    <t>check lib_path = lib_path or not</t>
+. preceeded by :::
+\b(?!base\b)\w+(?=::)</t>
+  </si>
+  <si>
+    <t>issue 82</t>
+  </si>
+  <si>
+    <t>in main fun, check that intern fun have the good args</t>
   </si>
 </sst>
 </file>
@@ -170,12 +177,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,12 +203,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -532,22 +551,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="14" width="9.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="13" width="9.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
@@ -576,20 +597,23 @@
         <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -617,14 +641,14 @@
         <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -636,43 +660,43 @@
       <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="O3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -683,7 +707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -723,22 +747,52 @@
       <c r="M9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -779,7 +833,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -787,7 +841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -795,7 +849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -803,7 +857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -811,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -819,15 +873,42 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F17" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -867,12 +948,12 @@
       <c r="M18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="O18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -885,31 +966,31 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F23" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
.has_odd_number_of_quotes BACKBONE v10.7 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4D431-A5FB-4784-AC33-C527C3378824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD85E1-AC93-4661-BFB0-588C91D8C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -554,7 +554,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -853,7 +853,34 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.in_quotes_replacement BACKBONE v10.7 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD85E1-AC93-4661-BFB0-588C91D8C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D38F3F3-9563-4CAD-B402-F049174CF6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -137,10 +137,6 @@
   <si>
     <t>78
 internal fun no arg_check -&gt; deal with ""</t>
-  </si>
-  <si>
-    <t>79
-required function fill in internal</t>
   </si>
   <si>
     <t>81
@@ -162,6 +158,10 @@
   </si>
   <si>
     <t>in main fun, check that intern fun have the good args</t>
+  </si>
+  <si>
+    <t>79
+required function writted in internal</t>
   </si>
 </sst>
 </file>
@@ -214,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -554,7 +554,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -579,34 +579,34 @@
         <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>24</v>
@@ -641,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>23</v>
@@ -657,7 +657,7 @@
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -668,7 +668,7 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -676,7 +676,7 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -684,7 +684,7 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -692,7 +692,7 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -703,7 +703,7 @@
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -762,7 +762,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -837,7 +837,7 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -845,7 +845,7 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -888,7 +888,7 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -896,7 +896,34 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -989,7 +1016,7 @@
       <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -997,7 +1024,7 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1005,7 +1032,7 @@
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1013,12 +1040,12 @@
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.in_parenthesis_replacement BACKBONE v10.7 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D38F3F3-9563-4CAD-B402-F049174CF6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A265673-4BF6-4910-96F6-086D05BCEC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -554,7 +554,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,34 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1011,9 +1038,6 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="2" t="s">

</xml_diff>

<commit_message>
.fun_args_pos BACKBONE v10.7 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A265673-4BF6-4910-96F6-086D05BCEC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74205319-5EC8-4E5F-B4FA-A28354BC357F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -554,7 +554,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -837,7 +837,34 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.all_args_here_fill and .all_args_here BACKBONE v10.7 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74205319-5EC8-4E5F-B4FA-A28354BC357F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF1A20-4C1D-4024-A5AD-23ABBEC7AE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Unit tests</t>
-  </si>
-  <si>
-    <t>compare with .colons_check_message</t>
   </si>
   <si>
     <t>BACKBONE v10.7</t>
@@ -203,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -213,9 +210,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,7 +548,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -573,40 +567,40 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>24</v>
@@ -641,9 +635,15 @@
         <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -696,14 +696,38 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -762,7 +786,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -872,7 +896,34 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -985,7 +1036,7 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="2" t="s">

</xml_diff>

<commit_message>
for all the functions with BACKBONE v10.7: intern fun have the good args
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACF1A20-4C1D-4024-A5AD-23ABBEC7AE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DFB97C-180F-4848-BEE3-EB20A1245CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="38">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -548,7 +548,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -646,6 +646,9 @@
       <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N2" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -730,6 +733,9 @@
       <c r="M8" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -771,6 +777,9 @@
       <c r="M9" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="O9" s="2" t="s">
         <v>23</v>
       </c>
@@ -815,6 +824,9 @@
       <c r="M10" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N10" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -856,6 +868,9 @@
       <c r="M11" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N11" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -891,6 +906,9 @@
       <c r="M12" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -926,6 +944,9 @@
       <c r="M13" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N13" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -961,6 +982,9 @@
       <c r="M14" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N14" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -996,6 +1020,9 @@
       <c r="M15" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N15" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1031,6 +1058,9 @@
       <c r="M16" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N16" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1066,6 +1096,9 @@
       <c r="M17" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="N17" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1105,6 +1138,9 @@
         <v>23</v>
       </c>
       <c r="M18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O18" s="2" t="s">

</xml_diff>

<commit_message>
arg_check BACKBONE v10.7 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DFB97C-180F-4848-BEE3-EB20A1245CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8E4450-AC5D-4334-932F-0226A8372760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="38">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -548,7 +548,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -657,10 +657,40 @@
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -679,7 +709,37 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1154,7 +1214,37 @@
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
get_message BACKBONE v11 and check TODO done except all_args_here because blocked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FB89DB-992D-4F11-8A00-157072A63B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC49AA6D-54EB-46CC-A9CD-D8807627DD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -101,9 +101,6 @@
     <t>report.R</t>
   </si>
   <si>
-    <t>BACKBONE v10.6</t>
-  </si>
-  <si>
     <t>all_args_here</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
   </si>
   <si>
     <t>Unit tests</t>
-  </si>
-  <si>
-    <t>BACKBONE v10.7</t>
   </si>
   <si>
     <t>71
@@ -159,6 +153,27 @@
   <si>
     <t>79
 required function writted in internal</t>
+  </si>
+  <si>
+    <t>BACKBONE v10.7
+default value
+NULL
+arg_check
+""
+not required sections</t>
+  </si>
+  <si>
+    <t>BACKBONE v11.0
+default value
+NULL
+arg_check
+""
+not required sections</t>
+  </si>
+  <si>
+    <t>ERROR
+stop(
+error_text_start</t>
   </si>
 </sst>
 </file>
@@ -545,736 +560,797 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="13" width="9.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="13" style="2" customWidth="1"/>
+    <col min="5" max="14" width="9.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>23</v>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>23</v>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>23</v>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="2" t="s">
-        <v>23</v>
+      <c r="H22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all internal and test-.pack_and_function_check test-.base_op_check with BACKBONE v12.1
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC49AA6D-54EB-46CC-A9CD-D8807627DD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF9F456-B514-4A99-8EC8-1AF4E5AB1041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="40">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -174,6 +174,14 @@
     <t>ERROR
 stop(
 error_text_start</t>
+  </si>
+  <si>
+    <t>BACKBONE v12.1
+default value
+NULL
+arg_check
+""
+not required sections</t>
   </si>
 </sst>
 </file>
@@ -560,25 +568,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="14" width="9.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="4" width="13.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" customWidth="1"/>
+    <col min="6" max="15" width="9.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
@@ -586,55 +594,55 @@
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
@@ -654,11 +662,11 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="M2" s="2" t="s">
         <v>22</v>
       </c>
@@ -668,8 +676,11 @@
       <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -715,25 +726,25 @@
       <c r="P3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
@@ -764,25 +775,25 @@
       <c r="O5" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
@@ -813,15 +824,18 @@
       <c r="O7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -854,8 +868,11 @@
       <c r="O8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -901,8 +918,11 @@
       <c r="P9" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -910,11 +930,11 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
@@ -945,8 +965,11 @@
       <c r="O10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -989,15 +1012,18 @@
       <c r="O11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1030,15 +1056,18 @@
       <c r="O12" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1071,15 +1100,18 @@
       <c r="O13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1112,15 +1144,18 @@
       <c r="O14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1153,15 +1188,18 @@
       <c r="O15" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -1194,15 +1232,18 @@
       <c r="O16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -1235,8 +1276,11 @@
       <c r="O17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1282,17 +1326,17 @@
       <c r="P18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1323,33 +1367,36 @@
       <c r="O19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="2" t="s">
+      <c r="I22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arg_check() all_args_here and all internal functions with backbone v13.1
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF9F456-B514-4A99-8EC8-1AF4E5AB1041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E8BCC-2EBF-4044-90D7-37AFC6D4E6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="40">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -176,7 +176,7 @@
 error_text_start</t>
   </si>
   <si>
-    <t>BACKBONE v12.1
+    <t>BACKBONE v13.1
 default value
 NULL
 arg_check
@@ -643,6 +643,9 @@
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1335,6 +1338,9 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">

</xml_diff>

<commit_message>
arg_check() all_args_here and all internal functions with backbone v14
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28E8BCC-2EBF-4044-90D7-37AFC6D4E6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E3ACB4-D5C2-42E8-A9E3-D834A04361C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="2130" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
 error_text_start</t>
   </si>
   <si>
-    <t>BACKBONE v13.1
+    <t>BACKBONE v14
 default value
 NULL
 arg_check
@@ -571,7 +571,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
backbone v15 for is_package_here
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4098E69F-C727-4220-8E8B-5626B1C914D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4892513A-D53C-4AAA-BB78-4BA9ECA75604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="14220" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="42">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -190,6 +190,12 @@
 arg_check
 ""
 not required sections</t>
+  </si>
+  <si>
+    <t>safer_check
+lib_path
+error_text
+manual in good order</t>
   </si>
 </sst>
 </file>
@@ -576,25 +582,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
     <col min="2" max="5" width="13.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13" style="2" customWidth="1"/>
-    <col min="7" max="16" width="9.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="7" width="13" style="2" customWidth="1"/>
+    <col min="8" max="17" width="9.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
@@ -611,43 +617,46 @@
         <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -663,9 +672,6 @@
       <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
@@ -682,11 +688,11 @@
         <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
@@ -696,8 +702,11 @@
       <c r="Q2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -713,9 +722,6 @@
       <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
@@ -749,23 +755,29 @@
       <c r="R3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -798,23 +810,26 @@
       <c r="Q5" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -847,8 +862,11 @@
       <c r="Q7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -861,9 +879,6 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H8" s="2" t="s">
         <v>22</v>
       </c>
@@ -894,8 +909,11 @@
       <c r="Q8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -905,12 +923,12 @@
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
@@ -944,8 +962,11 @@
       <c r="R9" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -955,12 +976,12 @@
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H10" s="2" t="s">
         <v>22</v>
       </c>
@@ -991,8 +1012,11 @@
       <c r="Q10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1002,12 +1026,12 @@
       <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1038,8 +1062,11 @@
       <c r="Q11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1049,7 +1076,7 @@
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1082,8 +1109,11 @@
       <c r="Q12" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1093,7 +1123,7 @@
       <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -1126,8 +1156,11 @@
       <c r="Q13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1137,7 +1170,7 @@
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1170,8 +1203,11 @@
       <c r="Q14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1181,7 +1217,7 @@
       <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -1214,8 +1250,11 @@
       <c r="Q15" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1264,7 @@
       <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -1258,8 +1297,11 @@
       <c r="Q16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1269,7 +1311,7 @@
       <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -1302,8 +1344,11 @@
       <c r="Q17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1313,12 +1358,12 @@
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1352,8 +1397,11 @@
       <c r="R18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1363,7 +1411,7 @@
       <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -1396,33 +1444,39 @@
       <c r="Q19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J23" s="2" t="s">
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all the functions with backbone v15+
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4892513A-D53C-4AAA-BB78-4BA9ECA75604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B3EF8B-D035-4F81-8D43-508EBD3C39C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="14220" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="20640" yWindow="-12990" windowWidth="28800" windowHeight="15450" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -155,33 +155,9 @@
 required function writted in internal</t>
   </si>
   <si>
-    <t>BACKBONE v10.7
-default value
-NULL
-arg_check
-""
-not required sections</t>
-  </si>
-  <si>
-    <t>BACKBONE v11.0
-default value
-NULL
-arg_check
-""
-not required sections</t>
-  </si>
-  <si>
     <t>ERROR
 stop(
 error_text_start</t>
-  </si>
-  <si>
-    <t>BACKBONE v14
-default value
-NULL
-arg_check
-""
-not required sections</t>
   </si>
   <si>
     <t>BACKBONE v15
@@ -582,88 +558,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="13.42578125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="13" style="2" customWidth="1"/>
-    <col min="8" max="17" width="9.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="13" style="2" customWidth="1"/>
+    <col min="5" max="14" width="9.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -672,6 +639,9 @@
       <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
@@ -682,7 +652,7 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>22</v>
@@ -691,29 +661,20 @@
         <v>22</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -722,6 +683,9 @@
       <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
@@ -749,28 +713,19 @@
       <c r="P3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -780,6 +735,12 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
@@ -804,34 +765,34 @@
       <c r="O5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
@@ -856,29 +817,23 @@
       <c r="O7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H8" s="2" t="s">
         <v>22</v>
       </c>
@@ -903,24 +858,15 @@
       <c r="O8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -929,6 +875,9 @@
       <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>22</v>
       </c>
@@ -956,31 +905,25 @@
       <c r="P9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>22</v>
@@ -1006,24 +949,15 @@
       <c r="O10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1032,6 +966,9 @@
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1056,29 +993,23 @@
       <c r="O11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1103,29 +1034,23 @@
       <c r="O12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1150,29 +1075,23 @@
       <c r="O13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1197,29 +1116,23 @@
       <c r="O14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1244,29 +1157,23 @@
       <c r="O15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1291,29 +1198,23 @@
       <c r="O16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1338,24 +1239,15 @@
       <c r="O17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1364,6 +1256,9 @@
       <c r="F18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1391,29 +1286,23 @@
       <c r="P18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Q18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1438,45 +1327,37 @@
       <c r="O19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
much advances in functions checking using TODO docs
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B3EF8B-D035-4F81-8D43-508EBD3C39C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7E092F-FD4D-4309-AB42-76F9EA4EE923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="-12990" windowWidth="28800" windowHeight="15450" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="39">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -132,9 +132,6 @@
   <si>
     <t>81
 internal errors number</t>
-  </si>
-  <si>
-    <t>nc</t>
   </si>
   <si>
     <t>check lib_path = lib_path or not</t>
@@ -149,15 +146,6 @@
   </si>
   <si>
     <t>in main fun, check that intern fun have the good args</t>
-  </si>
-  <si>
-    <t>79
-required function writted in internal</t>
-  </si>
-  <si>
-    <t>ERROR
-stop(
-error_text_start</t>
   </si>
   <si>
     <t>BACKBONE v15
@@ -172,6 +160,17 @@
 lib_path
 error_text
 manual in good order</t>
+  </si>
+  <si>
+    <t>"+check all arg_check"</t>
+  </si>
+  <si>
+    <t>ERROR
+tempo.cat &lt;-</t>
+  </si>
+  <si>
+    <t>79 80
+required function writted in internal</t>
   </si>
 </sst>
 </file>
@@ -560,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -578,19 +577,19 @@
   <sheetData>
     <row r="1" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>26</v>
@@ -608,16 +607,16 @@
         <v>28</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>23</v>
@@ -633,6 +632,9 @@
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
@@ -652,7 +654,7 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>22</v>
@@ -677,6 +679,9 @@
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
@@ -721,7 +726,37 @@
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -732,6 +767,9 @@
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
@@ -773,7 +811,34 @@
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -784,6 +849,9 @@
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
@@ -825,6 +893,9 @@
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
@@ -869,6 +940,9 @@
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
@@ -914,7 +988,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>22</v>
@@ -960,6 +1037,9 @@
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1001,6 +1081,9 @@
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1042,6 +1125,9 @@
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1083,6 +1169,9 @@
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1124,6 +1213,9 @@
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1165,6 +1257,9 @@
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1206,6 +1301,9 @@
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1250,6 +1348,9 @@
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1294,6 +1395,9 @@
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1335,7 +1439,34 @@
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1346,7 +1477,34 @@
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1357,7 +1515,34 @@
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arg_test: warning output updated fitting backbone v15
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7E092F-FD4D-4309-AB42-76F9EA4EE923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D300CCD-D82F-40D8-88BD-A80263EAB72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="40">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -171,6 +171,12 @@
   <si>
     <t>79 80
 required function writted in internal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    #### warning output
+use the backbone one
+ckeck no ini.warning.length
+warn.count</t>
   </si>
 </sst>
 </file>
@@ -557,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L22"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -571,11 +577,11 @@
     <col min="5" max="14" width="9.7109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" style="1" customWidth="1"/>
     <col min="18" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
@@ -621,8 +627,11 @@
       <c r="P1" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -669,7 +678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -719,7 +728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -760,7 +769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -804,7 +813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -842,7 +851,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -886,7 +895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -930,7 +939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -980,7 +989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1027,7 +1036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1118,7 +1127,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1171,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1206,7 +1215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
backbone v15.2 for all functions + TODO.xlsx well completed
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D300CCD-D82F-40D8-88BD-A80263EAB72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF589793-B93B-43EF-9333-9B07E4544BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="44">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>Unit tests</t>
   </si>
   <si>
     <t>71
@@ -137,15 +134,29 @@
     <t>check lib_path = lib_path or not</t>
   </si>
   <si>
-    <t>80
-. preceeded by :::
-\b(?!base\b)\w+(?=::)</t>
-  </si>
-  <si>
     <t>issue 82</t>
   </si>
   <si>
     <t>in main fun, check that intern fun have the good args</t>
+  </si>
+  <si>
+    <t>safer_check
+lib_path
+error_text
+manual in good order</t>
+  </si>
+  <si>
+    <t>"+check all arg_check"</t>
+  </si>
+  <si>
+    <t>ERROR
+tempo.cat &lt;-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    #### warning output
+use the backbone one
+ckeck no ini.warning.length
+warn.count</t>
   </si>
   <si>
     <t>BACKBONE v15
@@ -153,30 +164,37 @@
 NULL
 arg_check
 ""
-not required sections</t>
-  </si>
-  <si>
-    <t>safer_check
-lib_path
-error_text
-manual in good order</t>
-  </si>
-  <si>
-    <t>"+check all arg_check"</t>
-  </si>
-  <si>
-    <t>ERROR
-tempo.cat &lt;-</t>
-  </si>
-  <si>
-    <t>79 80
+not required sections
+warning before output</t>
+  </si>
+  <si>
+    <t>data1 argument -&gt; data
+because protected by no arg value section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backbone v15.2: 
+in internal functions
+error_text argument with no value but comment that no tracable error message returned </t>
+  </si>
+  <si>
+    <t>Unit tests
+backbone v15.2</t>
+  </si>
+  <si>
+    <t>backbone v15.2: warning before output</t>
+  </si>
+  <si>
+    <t>79
 required function writted in internal</t>
   </si>
   <si>
-    <t xml:space="preserve">    #### warning output
-use the backbone one
-ckeck no ini.warning.length
-warn.count</t>
+    <t>80
+. preceeded by :::
+\b(?!base\b)\w+(?=::)
+do it after colons_check</t>
+  </si>
+  <si>
+    <t>colons_check</t>
   </si>
 </sst>
 </file>
@@ -563,75 +581,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="14" width="9.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="6.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" customWidth="1"/>
+    <col min="6" max="15" width="9.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="2"/>
+    <col min="21" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -668,17 +701,29 @@
       <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -715,9 +760,6 @@
       <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N3" s="2" t="s">
         <v>22</v>
       </c>
@@ -727,8 +769,23 @@
       <c r="P3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -736,10 +793,10 @@
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
@@ -768,17 +825,32 @@
       <c r="N4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
@@ -803,26 +875,35 @@
       <c r="L5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
@@ -850,17 +931,32 @@
       <c r="N6" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
@@ -885,26 +981,35 @@
       <c r="L7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
@@ -929,17 +1034,29 @@
       <c r="L8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -976,9 +1093,6 @@
       <c r="L9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N9" s="2" t="s">
         <v>22</v>
       </c>
@@ -988,8 +1102,23 @@
       <c r="P9" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -997,10 +1126,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>22</v>
@@ -1026,17 +1155,29 @@
       <c r="L10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1073,26 +1214,35 @@
       <c r="L11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1117,26 +1267,35 @@
       <c r="L12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1161,26 +1320,35 @@
       <c r="L13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1205,26 +1373,35 @@
       <c r="L14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1249,26 +1426,35 @@
       <c r="L15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1293,26 +1479,35 @@
       <c r="L16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1337,17 +1532,29 @@
       <c r="L17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1384,9 +1591,6 @@
       <c r="L18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1396,17 +1600,29 @@
       <c r="P18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1431,26 +1647,35 @@
       <c r="L19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1478,17 +1703,32 @@
       <c r="N20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1516,17 +1756,32 @@
       <c r="N21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1552,6 +1807,24 @@
         <v>22</v>
       </c>
       <c r="N22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all functions ok with colons checking
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF589793-B93B-43EF-9333-9B07E4544BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D999A8E6-08C1-4DC8-9A0D-8633B8B0459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="44">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -584,7 +584,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>33</v>
@@ -851,6 +851,9 @@
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
@@ -904,6 +907,9 @@
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
@@ -957,6 +963,9 @@
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1010,6 +1019,9 @@
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>30</v>
@@ -1243,6 +1255,9 @@
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1296,6 +1311,9 @@
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1349,6 +1367,9 @@
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1402,6 +1423,9 @@
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1455,6 +1479,9 @@
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1508,6 +1535,9 @@
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1623,6 +1653,9 @@
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1676,6 +1709,9 @@
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1729,6 +1765,9 @@
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1780,6 +1819,9 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="2" t="s">

</xml_diff>

<commit_message>
issue 64 probably solved
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D999A8E6-08C1-4DC8-9A0D-8633B8B0459F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B304C1-BE01-4088-A015-C447CEC0B961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="44">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -188,13 +188,12 @@
 required function writted in internal</t>
   </si>
   <si>
+    <t>colons_check</t>
+  </si>
+  <si>
     <t>80
-. preceeded by :::
-\b(?!base\b)\w+(?=::)
+\b(?!(base|utils|grDevices|graphics)\b)\w+(?=::)
 do it after colons_check</t>
-  </si>
-  <si>
-    <t>colons_check</t>
   </si>
 </sst>
 </file>
@@ -584,7 +583,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -607,7 +606,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>21</v>
@@ -637,7 +636,7 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>41</v>
@@ -701,6 +700,9 @@
       <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
@@ -760,6 +762,9 @@
       <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N3" s="2" t="s">
         <v>22</v>
       </c>
@@ -822,6 +827,9 @@
       <c r="L4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N4" s="2" t="s">
         <v>22</v>
       </c>
@@ -878,6 +886,9 @@
       <c r="L5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
@@ -934,6 +945,9 @@
       <c r="L6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N6" s="2" t="s">
         <v>22</v>
       </c>
@@ -990,6 +1004,9 @@
       <c r="L7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1046,6 +1063,9 @@
       <c r="L8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1105,6 +1125,9 @@
       <c r="L9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1167,6 +1190,9 @@
       <c r="L10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M10" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1226,6 +1252,9 @@
       <c r="L11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1282,6 +1311,9 @@
       <c r="L12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1338,6 +1370,9 @@
       <c r="L13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1394,6 +1429,9 @@
       <c r="L14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1450,6 +1488,9 @@
       <c r="L15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1506,6 +1547,9 @@
       <c r="L16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1562,6 +1606,9 @@
       <c r="L17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M17" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1621,6 +1668,9 @@
       <c r="L18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1680,6 +1730,9 @@
       <c r="L19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1736,6 +1789,9 @@
       <c r="L20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1792,6 +1848,9 @@
       <c r="L21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M21" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="N21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1846,6 +1905,9 @@
         <v>22</v>
       </c>
       <c r="L22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N22" s="2" t="s">

</xml_diff>

<commit_message>
backbone v15.3 in all functions
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFD2595-5942-461D-ABD3-3A6F7A3DA17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727D4FB6-34EB-46A0-911B-AFB716101566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="45">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -586,7 +586,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -730,6 +730,9 @@
       <c r="U2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -795,6 +798,9 @@
       <c r="U3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -857,6 +863,9 @@
       <c r="U4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -916,6 +925,9 @@
       <c r="U5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V5" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -975,6 +987,9 @@
       <c r="U6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1034,6 +1049,9 @@
       <c r="U7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V7" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1093,6 +1111,9 @@
       <c r="U8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V8" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1158,6 +1179,9 @@
       <c r="U9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V9" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1220,6 +1244,9 @@
       <c r="U10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V10" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1282,6 +1309,9 @@
       <c r="U11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V11" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1341,6 +1371,9 @@
       <c r="U12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1400,6 +1433,9 @@
       <c r="U13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V13" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1459,6 +1495,9 @@
       <c r="U14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V14" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1518,6 +1557,9 @@
       <c r="U15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="V15" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1577,8 +1619,11 @@
       <c r="U16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1636,8 +1681,11 @@
       <c r="U17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1701,8 +1749,11 @@
       <c r="U18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1760,8 +1811,11 @@
       <c r="U19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1819,8 +1873,11 @@
       <c r="U20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1878,8 +1935,11 @@
       <c r="U21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1935,6 +1995,9 @@
         <v>22</v>
       </c>
       <c r="U22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all_args_here now skips as.environment
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727D4FB6-34EB-46A0-911B-AFB716101566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B96BB78-A93C-4E07-8B09-826FDFD74ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="44">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>check lib_path = lib_path or not</t>
-  </si>
-  <si>
-    <t>issue 82</t>
   </si>
   <si>
     <t>in main fun, check that intern fun have the good args</t>
@@ -586,7 +583,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -606,22 +603,22 @@
   <sheetData>
     <row r="1" spans="1:22" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>25</v>
@@ -639,34 +636,34 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -813,7 +810,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
@@ -877,6 +874,9 @@
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
all_args_here and env_check updated
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B96BB78-A93C-4E07-8B09-826FDFD74ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0391FA70-55AE-43F1-B4E7-09F11A44569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="45">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>backbone v15.3</t>
+  </si>
+  <si>
+    <t>check examples</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -595,13 +598,13 @@
     <col min="5" max="5" width="13" style="2" customWidth="1"/>
     <col min="6" max="15" width="9.7109375" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" style="1" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" style="2"/>
-    <col min="21" max="16384" width="11.42578125" style="1"/>
+    <col min="17" max="18" width="9.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="11.42578125" style="2"/>
+    <col min="22" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -650,23 +653,26 @@
       <c r="Q1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -715,9 +721,6 @@
       <c r="P2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S2" s="2" t="s">
         <v>22</v>
       </c>
@@ -730,8 +733,11 @@
       <c r="V2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -783,9 +789,6 @@
       <c r="Q3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S3" s="2" t="s">
         <v>22</v>
       </c>
@@ -798,8 +801,11 @@
       <c r="V3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -848,9 +854,6 @@
       <c r="P4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S4" s="2" t="s">
         <v>22</v>
       </c>
@@ -863,8 +866,11 @@
       <c r="V4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -913,9 +919,6 @@
       <c r="P5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S5" s="2" t="s">
         <v>22</v>
       </c>
@@ -928,8 +931,11 @@
       <c r="V5" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -939,6 +945,9 @@
       <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
@@ -990,8 +999,11 @@
       <c r="V6" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1037,9 +1049,6 @@
       <c r="P7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1052,8 +1061,11 @@
       <c r="V7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1099,9 +1111,6 @@
       <c r="P8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1114,8 +1123,11 @@
       <c r="V8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1167,9 +1179,6 @@
       <c r="Q9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1182,8 +1191,11 @@
       <c r="V9" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1232,9 +1244,6 @@
       <c r="P10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1247,8 +1256,11 @@
       <c r="V10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1297,9 +1309,6 @@
       <c r="P11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1312,8 +1321,11 @@
       <c r="V11" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1359,9 +1371,6 @@
       <c r="P12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1374,8 +1383,11 @@
       <c r="V12" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1421,9 +1433,6 @@
       <c r="P13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1436,8 +1445,11 @@
       <c r="V13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1483,9 +1495,6 @@
       <c r="P14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1498,8 +1507,11 @@
       <c r="V14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1545,9 +1557,6 @@
       <c r="P15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1560,8 +1569,11 @@
       <c r="V15" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1607,9 +1619,6 @@
       <c r="P16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1622,8 +1631,11 @@
       <c r="V16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1669,9 +1681,6 @@
       <c r="P17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1684,8 +1693,11 @@
       <c r="V17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1737,9 +1749,6 @@
       <c r="Q18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R18" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1752,8 +1761,11 @@
       <c r="V18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1799,9 +1811,6 @@
       <c r="P19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1814,8 +1823,11 @@
       <c r="V19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1861,9 +1873,6 @@
       <c r="P20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R20" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1876,8 +1885,11 @@
       <c r="V20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1923,9 +1935,6 @@
       <c r="P21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R21" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1938,8 +1947,11 @@
       <c r="V21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1985,9 +1997,6 @@
       <c r="P22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R22" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="S22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1998,6 +2007,9 @@
         <v>22</v>
       </c>
       <c r="V22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
get_message with all its arguments
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0391FA70-55AE-43F1-B4E7-09F11A44569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868E2EBE-C1F9-4BEC-97D2-8532688F3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="45">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -586,7 +586,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1013,6 +1013,9 @@
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1047,6 +1050,9 @@
         <v>22</v>
       </c>
       <c r="P7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S7" s="2" t="s">

</xml_diff>

<commit_message>
.all_args_here_fill bug fixed so that no unexpected = in the MISSING_ARG column of the output
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868E2EBE-C1F9-4BEC-97D2-8532688F3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F984ED-AFF3-4022-A901-22DFB6C02E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
all args here for is_function_here and is_package_here, and is_python_package_here removed because broken
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F984ED-AFF3-4022-A901-22DFB6C02E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC9109B-9CFD-44B6-82D7-A9B1DD009EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="45">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -586,7 +586,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1781,6 +1781,9 @@
       <c r="C19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1815,6 +1818,9 @@
         <v>22</v>
       </c>
       <c r="P19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S19" s="2" t="s">
@@ -1843,6 +1849,9 @@
       <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1877,6 +1886,9 @@
         <v>22</v>
       </c>
       <c r="P20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S20" s="2" t="s">
@@ -1903,6 +1915,9 @@
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E21" s="2" t="s">

</xml_diff>

<commit_message>
attempt to add the detection of 'function<-'() in all_args_here
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC9109B-9CFD-44B6-82D7-A9B1DD009EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB6F42E-D58A-463C-B586-377012501D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="46">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -174,10 +174,6 @@
 error_text argument with no value but comment that no tracable error message returned </t>
   </si>
   <si>
-    <t>Unit tests
-backbone v15.2</t>
-  </si>
-  <si>
     <t>backbone v15.2: warning before output</t>
   </si>
   <si>
@@ -197,16 +193,29 @@
   </si>
   <si>
     <t>check examples</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>Unit tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -248,6 +257,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +598,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -609,7 +621,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>21</v>
@@ -639,10 +651,10 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>29</v>
@@ -651,16 +663,16 @@
         <v>30</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>37</v>
@@ -669,7 +681,7 @@
         <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1956,6 +1968,9 @@
       <c r="P21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R21" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="S21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1982,6 +1997,9 @@
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2016,6 +2034,9 @@
         <v>22</v>
       </c>
       <c r="P22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S22" s="2" t="s">

</xml_diff>

<commit_message>
.all_args_here_fill() with all args and examples checked
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB6F42E-D58A-463C-B586-377012501D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3F4119-8359-4DF1-9622-E03545090905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="46">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -598,7 +598,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1093,6 +1093,9 @@
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1127,6 +1130,9 @@
         <v>22</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S8" s="2" t="s">

</xml_diff>

<commit_message>
.extract_all_fun_names() with all args
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3F4119-8359-4DF1-9622-E03545090905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D590CD70-8A52-43D9-A7AA-9540ABAD96FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="46">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -598,7 +598,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1359,6 +1359,9 @@
       <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1393,6 +1396,9 @@
         <v>22</v>
       </c>
       <c r="P12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S12" s="2" t="s">

</xml_diff>

<commit_message>
.in_quotes_replacement() with all args
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D590CD70-8A52-43D9-A7AA-9540ABAD96FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD6A5D-14CF-4D62-8FEE-8A4FFD209FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="46">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -598,7 +598,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1613,6 +1613,9 @@
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1647,6 +1650,9 @@
         <v>22</v>
       </c>
       <c r="P16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S16" s="2" t="s">

</xml_diff>

<commit_message>
.in_parenthesis_replacement() with all args
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD6A5D-14CF-4D62-8FEE-8A4FFD209FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B9F66C-ADB8-4880-860F-030FADD0C002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="46">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -598,7 +598,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1551,6 +1551,9 @@
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1585,6 +1588,9 @@
         <v>22</v>
       </c>
       <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S15" s="2" t="s">

</xml_diff>

<commit_message>
arg_test checked for arg_check
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B9F66C-ADB8-4880-860F-030FADD0C002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7D5624-52A9-4BFF-9DCE-F7399CEC230A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="45">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -141,9 +141,6 @@
 lib_path
 error_text
 manual in good order</t>
-  </si>
-  <si>
-    <t>"+check all arg_check"</t>
   </si>
   <si>
     <t>ERROR
@@ -598,7 +595,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -618,10 +615,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>21</v>
@@ -633,7 +630,7 @@
         <v>28</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>25</v>
@@ -651,10 +648,10 @@
         <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>29</v>
@@ -663,25 +660,25 @@
         <v>30</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -827,9 +824,6 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1993,7 +1987,7 @@
         <v>22</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
.has_odd_number_of_quotes() with all args
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7D5624-52A9-4BFF-9DCE-F7399CEC230A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C2037A-5764-43D8-8569-4D396E3C71AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="45">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -595,7 +595,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1421,6 +1421,9 @@
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1455,6 +1458,9 @@
         <v>22</v>
       </c>
       <c r="P13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S13" s="2" t="s">
@@ -1483,6 +1489,9 @@
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1517,6 +1526,9 @@
         <v>22</v>
       </c>
       <c r="P14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S14" s="2" t="s">

</xml_diff>

<commit_message>
package rebuilt to test code balise
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463E698B-F654-4023-A3F2-076477507398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE62F4F-6FD8-4639-92F1-09855DC89720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="25095" windowHeight="15585" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="46">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Unit tests</t>
+  </si>
+  <si>
+    <t>check help page</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -257,6 +260,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -613,7 +622,7 @@
     <col min="22" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
@@ -680,8 +689,11 @@
       <c r="W1" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -730,6 +742,9 @@
       <c r="P2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="S2" s="2" t="s">
         <v>22</v>
       </c>
@@ -746,7 +761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -798,6 +813,9 @@
       <c r="Q3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="S3" s="2" t="s">
         <v>22</v>
       </c>
@@ -814,7 +832,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -876,7 +894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -925,6 +943,9 @@
       <c r="P5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="S5" s="2" t="s">
         <v>22</v>
       </c>
@@ -941,7 +962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1145,7 +1166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1278,7 +1299,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1343,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1479,7 +1500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1547,7 +1568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1615,7 +1636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1955,71 +1976,72 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:23" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="4"/>
       <c r="R21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="S21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="W21" s="2" t="s">
+      <c r="S21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="W21" s="4" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all examples checked except arg_test
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E5CB86-2686-4B9D-B79A-306477DC7D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9766409A-7F91-40BC-AB27-9CEB3BEF2E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="25095" windowHeight="15585" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="49">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -199,6 +199,20 @@
   </si>
   <si>
     <t>check help page</t>
+  </si>
+  <si>
+    <t>help pages
+use \code{}</t>
+  </si>
+  <si>
+    <t>help pages
+authors with html mail
+\href{https://www.example.com}{link text}</t>
+  </si>
+  <si>
+    <t>help pages
+other functions
+\link{try}</t>
   </si>
 </sst>
 </file>
@@ -601,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A2B6C9-DACA-4606-B471-C75D7DA26424}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -622,7 +636,7 @@
     <col min="22" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
@@ -692,8 +706,17 @@
       <c r="X1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -760,8 +783,11 @@
       <c r="W2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -831,8 +857,11 @@
       <c r="W3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -893,8 +922,11 @@
       <c r="W4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -961,8 +993,11 @@
       <c r="W5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z5" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1029,8 +1064,11 @@
       <c r="W6" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1097,8 +1135,11 @@
       <c r="W7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z7" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1165,8 +1206,11 @@
       <c r="W8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z8" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1236,8 +1280,11 @@
       <c r="W9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z9" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1286,6 +1333,9 @@
       <c r="P10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R10" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="S10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1301,8 +1351,11 @@
       <c r="W10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z10" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1351,6 +1404,9 @@
       <c r="P11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="S11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1366,8 +1422,11 @@
       <c r="W11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z11" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1434,8 +1493,11 @@
       <c r="W12" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1502,8 +1564,11 @@
       <c r="W13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z13" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1570,8 +1635,11 @@
       <c r="W14" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z14" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1638,8 +1706,11 @@
       <c r="W15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z15" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1706,8 +1777,11 @@
       <c r="W16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z16" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1774,8 +1848,11 @@
       <c r="W17" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z17" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1827,6 +1904,9 @@
       <c r="Q18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="R18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="S18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1842,8 +1922,11 @@
       <c r="W18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z18" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1910,8 +1993,11 @@
       <c r="W19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z19" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1978,8 +2064,11 @@
       <c r="W20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Z20" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -2047,8 +2136,9 @@
       <c r="W21" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="Z21" s="4"/>
     </row>
-    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -2113,6 +2203,9 @@
         <v>22</v>
       </c>
       <c r="W22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z22" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arg_test with bug solved for tempo.cat
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9766409A-7F91-40BC-AB27-9CEB3BEF2E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20151428-035E-4FDC-A637-DF6723065CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
+    <workbookView xWindow="19090" yWindow="-16300" windowWidth="38620" windowHeight="21100" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="49">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -618,7 +618,7 @@
   <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -871,6 +871,9 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
@@ -905,6 +908,9 @@
         <v>22</v>
       </c>
       <c r="P4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="S4" s="2" t="s">

</xml_diff>

<commit_message>
.noclean_functions() with unit test
</commit_message>
<xml_diff>
--- a/dev/TODO_backbone_all_args.xlsx
+++ b/dev/TODO_backbone_all_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmillot\Documents\Git_projects\safer-r\saferDev\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF62464-176D-48CC-B576-1474B5D7CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882E7AB7-914E-44A2-A946-B5E76AF68632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{07E7905C-C0FC-435A-9AE4-BD70C30EB32A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="49">
   <si>
     <t>all_args_here.R</t>
   </si>
@@ -618,7 +618,7 @@
   <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1410,6 +1410,9 @@
       <c r="P11" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="Q11" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="R11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1695,6 +1698,9 @@
         <v>22</v>
       </c>
       <c r="P15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="R15" s="2" t="s">

</xml_diff>